<commit_message>
remove medicine names with slash in them
</commit_message>
<xml_diff>
--- a/research results/Two Level Numbers.xlsx
+++ b/research results/Two Level Numbers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SVM - Obesity" sheetId="4" r:id="rId1"/>
@@ -523,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -931,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
code for confusion matrix
</commit_message>
<xml_diff>
--- a/research results/Two Level Numbers.xlsx
+++ b/research results/Two Level Numbers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="SVM - Obesity" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
   <si>
     <t>Min Preprocessing</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>ngram(1,3)</t>
+  </si>
+  <si>
+    <t>Tf-Idf</t>
   </si>
 </sst>
 </file>
@@ -523,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +717,9 @@
       <c r="B22" s="12">
         <v>95.3</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1">
+        <v>94.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -726,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +870,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -931,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>